<commit_message>
fix: bug in views column
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="337">
   <si>
     <t>Title</t>
   </si>
@@ -28,670 +28,757 @@
     <t>HIKARU'S REAL THOUGHTS ABOUT LEVY REVEALED 😞 | LIE DETECTOR CHESS</t>
   </si>
   <si>
-    <t>391K просмотров</t>
-  </si>
-  <si>
-    <t>40:18</t>
+    <t>426K просмотров</t>
+  </si>
+  <si>
+    <t>40 минут 18 секунд</t>
   </si>
   <si>
     <t>Chess Prodigy Bodhana Sivananadan Meets Judit Polgar, The Greatest Woman Chess Player Of All Time!</t>
   </si>
   <si>
-    <t>2 дня назад</t>
+    <t>22K просмотров</t>
   </si>
   <si>
     <t>3 Minutes Of Hikaru Premoving Checkmate</t>
   </si>
   <si>
-    <t>22K просмотров</t>
-  </si>
-  <si>
-    <t>20:07</t>
+    <t>32K просмотров</t>
+  </si>
+  <si>
+    <t>20 минут 7 секунд</t>
   </si>
   <si>
     <t>GRANDMASTERS GUESS CHESS POSITIONS WITHOUT SEEING THE PIECES</t>
   </si>
   <si>
-    <t>7 дней назад</t>
+    <t>296K просмотров</t>
   </si>
   <si>
     <t>THE WORST CHESS ADVICE?! GM REACTS!</t>
   </si>
   <si>
-    <t>31K просмотров</t>
-  </si>
-  <si>
-    <t>3:43</t>
+    <t>103K просмотров</t>
+  </si>
+  <si>
+    <t>3 минуты 43 секунды</t>
   </si>
   <si>
     <t>The BEST Moments From The Norway Chess Confessional Booth!</t>
   </si>
   <si>
-    <t>9 дней назад</t>
+    <t>53K просмотров</t>
   </si>
   <si>
     <t>MAGNUS, HIKARU, VISHY RANK HILARIOUS MEME CHESS OPENINGS!</t>
   </si>
   <si>
-    <t>292K просмотров</t>
-  </si>
-  <si>
-    <t>10:07</t>
+    <t>197K просмотров</t>
+  </si>
+  <si>
+    <t>10 минут 7 секунд</t>
   </si>
   <si>
     <t>MAGNUS SHOCKED BY THE END OF HIKARU VS. PRAGG!</t>
   </si>
   <si>
-    <t>2 недели назад</t>
+    <t>137K просмотров</t>
   </si>
   <si>
     <t>THIS GAME DECIDED THE CHAMPION OF NORWAY CHESS!</t>
   </si>
   <si>
-    <t>103K просмотров</t>
-  </si>
-  <si>
-    <t>12:30</t>
+    <t>85K просмотров</t>
+  </si>
+  <si>
+    <t>12 минут 30 секунд</t>
   </si>
   <si>
     <t>MAGNUS GETS INTO A CRAZY TIME SCRAMBLE VS ALIREZA</t>
   </si>
   <si>
-    <t>3 недели назад</t>
+    <t>57K просмотров</t>
   </si>
   <si>
     <t>HOW PRAGG BEAT THE WORLD CHAMPION</t>
   </si>
   <si>
-    <t>53K просмотров</t>
-  </si>
-  <si>
-    <t>6:03</t>
+    <t>19K просмотров</t>
+  </si>
+  <si>
+    <t>6 минут 3 секунды</t>
   </si>
   <si>
     <t>HIKARU THRILLED AFTER BIG WIN VS MAGNUS IN ARMAGEDDON</t>
   </si>
   <si>
+    <t>94K просмотров</t>
+  </si>
+  <si>
     <t>HIKARU VS MAGNUS: WILDEST. GAME. EVER!</t>
   </si>
   <si>
+    <t>233K просмотров</t>
+  </si>
+  <si>
+    <t>4 минуты 40 секунд</t>
+  </si>
+  <si>
+    <t>HIKARU vs #3 IN THE WORLD!!!</t>
+  </si>
+  <si>
+    <t>12K просмотров</t>
+  </si>
+  <si>
+    <t>FABIANO OUTPLAYS STOCKFISH IN ANALYSIS!</t>
+  </si>
+  <si>
+    <t>93K просмотров</t>
+  </si>
+  <si>
+    <t>29 минут 7 секунд</t>
+  </si>
+  <si>
+    <t>HIKARU ON BREAKING THE 2800 BARRIER IN CLASSICAL CHESS</t>
+  </si>
+  <si>
+    <t>150K просмотров</t>
+  </si>
+  <si>
+    <t>MAGNUS ON THE ODDS OF LOSING HIS WORLD NO.1 SPOT</t>
+  </si>
+  <si>
+    <t>180K просмотров</t>
+  </si>
+  <si>
+    <t>16 минут 52 секунды</t>
+  </si>
+  <si>
+    <t>PRAGG BEATS MAGNUS FOR THE 1ST TIME IN CLASSICAL CHESS!</t>
+  </si>
+  <si>
+    <t>185K просмотров</t>
+  </si>
+  <si>
+    <t>Accused of Cheating by World Champions, Can He Prove Them Wrong?</t>
+  </si>
+  <si>
+    <t>139K просмотров</t>
+  </si>
+  <si>
+    <t>17 минут 26 секунд</t>
+  </si>
+  <si>
+    <t>MAGNUS VS HIKARU ARMAGEDDON!!</t>
+  </si>
+  <si>
+    <t>38K просмотров</t>
+  </si>
+  <si>
+    <t>HIKARU VS. FABI IN WILD ARMAGEDDON!</t>
+  </si>
+  <si>
+    <t>9 минут 38 секунд</t>
+  </si>
+  <si>
+    <t>🚨 MAGNUS VS DING! CURRENT VS FORMER WORLD CHAMP! ARMAGEDDON TIEBREAKER! 🚨</t>
+  </si>
+  <si>
+    <t>43K просмотров</t>
+  </si>
+  <si>
+    <t>Can These Chess Grandmasters Ace This Simple Spelling Test??</t>
+  </si>
+  <si>
+    <t>23K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 7 секунд</t>
+  </si>
+  <si>
+    <t>Magnus and Hikaru Face Off In A Historic Battle</t>
+  </si>
+  <si>
+    <t>The WILD Final Game Between Magnus And Alireza!</t>
+  </si>
+  <si>
+    <t>69K просмотров</t>
+  </si>
+  <si>
+    <t>16 минут 48 секунд</t>
+  </si>
+  <si>
+    <t>Alireza: "I was lucky that Magnus got so tilted after game 4"</t>
+  </si>
+  <si>
+    <t>39K просмотров</t>
+  </si>
+  <si>
+    <t>Vishy Answers The Web's Most Searched Questions!</t>
+  </si>
+  <si>
+    <t>82K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 59 секунд</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen: "I knew if I won this match I would have two days off"</t>
+  </si>
+  <si>
+    <t>77K просмотров</t>
+  </si>
+  <si>
+    <t>We Combined Disc Golf and Giant Chess!</t>
+  </si>
+  <si>
+    <t>22 минуты 41 секунда</t>
+  </si>
+  <si>
+    <t>5 Minutes Of Grandmasters Losing Their Minds To Crazy Moves</t>
+  </si>
+  <si>
+    <t>201K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus Forced to Answer Tough Personal Questions 🌶️ | LIE DETECTOR CHESS</t>
+  </si>
+  <si>
+    <t>949K просмотров</t>
+  </si>
+  <si>
+    <t>22 минуты 17 секунд</t>
+  </si>
+  <si>
+    <t>They Left Everything On The Board | Nepo vs. Fabi | Candidates 2024</t>
+  </si>
+  <si>
+    <t>90K просмотров</t>
+  </si>
+  <si>
+    <t>Vaishali Opens Up About The Pressures of Chess Stardom In India</t>
+  </si>
+  <si>
+    <t>55K просмотров</t>
+  </si>
+  <si>
+    <t>12 минут 31 секунда</t>
+  </si>
+  <si>
+    <t>Every Move From Pragg vs. Fabi | Candidates 2024 Round 13</t>
+  </si>
+  <si>
+    <t>9,8K просмотров</t>
+  </si>
+  <si>
+    <t>Final Heart-stopping Moments From Gukesh vs. Alireza | Candidates 2024</t>
+  </si>
+  <si>
+    <t>72K просмотров</t>
+  </si>
+  <si>
+    <t>11 минут 31 секунда</t>
+  </si>
+  <si>
+    <t>Every Move from Hikaru vs. Alireza | Candidates 2024 Round 12</t>
+  </si>
+  <si>
+    <t>24K просмотров</t>
+  </si>
+  <si>
+    <t>GothamChess And Vidit Dive Into The Emotions Of The Candidates!</t>
+  </si>
+  <si>
+    <t>83K просмотров</t>
+  </si>
+  <si>
+    <t>21 минута 46 секунд</t>
+  </si>
+  <si>
+    <t>What An Endgame 🤯 | Vidit vs. Nepo</t>
+  </si>
+  <si>
+    <t>62K просмотров</t>
+  </si>
+  <si>
+    <t>Did GothamChess And Nijat Just Become Best Friends?!</t>
+  </si>
+  <si>
+    <t>73K просмотров</t>
+  </si>
+  <si>
+    <t>15 минут 38 секунд</t>
+  </si>
+  <si>
+    <t>Chess is BRUTAL! | Alireza vs. Gukesh | Candidates 2024</t>
+  </si>
+  <si>
+    <t>98K просмотров</t>
+  </si>
+  <si>
+    <t>The Brilliant Final Moments of Hikaru vs. Nepo | Candidates 2024</t>
+  </si>
+  <si>
+    <t>97K просмотров</t>
+  </si>
+  <si>
+    <t>16 минут 53 секунды</t>
+  </si>
+  <si>
+    <t>The Stressful Final 5 Minutes Of Vidit vs. Alireza | Candidates 2024</t>
+  </si>
+  <si>
+    <t>41K просмотров</t>
+  </si>
+  <si>
+    <t>GothamChess and Pragg Finally Meet in Exclusive Interview!</t>
+  </si>
+  <si>
+    <t>238K просмотров</t>
+  </si>
+  <si>
+    <t>17 минут 44 секунды</t>
+  </si>
+  <si>
+    <t>Nepo Vs. Pragg | Game 6 | Candidates 2024</t>
+  </si>
+  <si>
+    <t>The Wild Final 10 Minutes Of Hikaru vs. Alireza | Candidates 2024</t>
+  </si>
+  <si>
+    <t>199K просмотров</t>
+  </si>
+  <si>
+    <t>4 минуты 18 секунд</t>
+  </si>
+  <si>
+    <t>Vishy's Exclusive Dinner with Indian Candidates ft. Pragg, Gukesh, Vaishali, Humpy</t>
+  </si>
+  <si>
+    <t>758K просмотров</t>
+  </si>
+  <si>
+    <t>Fabiano's Fight To Be The No. 1 Chess Player In The World</t>
+  </si>
+  <si>
+    <t>38 минут 8 секунд</t>
+  </si>
+  <si>
+    <t>Chess.com but it's IRL</t>
+  </si>
+  <si>
+    <t>Vaishali's Dreams Of Becoming A Chess World Champion</t>
+  </si>
+  <si>
+    <t>14 минут 46 секунд</t>
+  </si>
+  <si>
+    <t>We Finally Updated Chess (APRIL FOOLS!)</t>
+  </si>
+  <si>
+    <t>159K просмотров</t>
+  </si>
+  <si>
+    <t>This Impossible Puzzle Stumped 99% Of Chess.com Users!</t>
+  </si>
+  <si>
+    <t>30K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 12 секунд</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen Ranks The Candidates Players! 🌶️</t>
+  </si>
+  <si>
+    <t>1M просмотров</t>
+  </si>
+  <si>
+    <t>The Craziest Moments From The Candidates!</t>
+  </si>
+  <si>
+    <t>112K просмотров</t>
+  </si>
+  <si>
+    <t>Gukesh Fights Back Against Anish Giri To Find A Huge Win!</t>
+  </si>
+  <si>
+    <t>16K просмотров</t>
+  </si>
+  <si>
+    <t>Can This 17-Year-Old Make Chess History and Win a Ticket to the World Championship?</t>
+  </si>
+  <si>
+    <t>28K просмотров</t>
+  </si>
+  <si>
+    <t>7 минут 24 секунды</t>
+  </si>
+  <si>
+    <t>Game 1 Of The Drama Filled Match Between Anish Giri and Gukesh</t>
+  </si>
+  <si>
+    <t>20K просмотров</t>
+  </si>
+  <si>
+    <t>The Chess Game That Changed Wesley So's Life</t>
+  </si>
+  <si>
+    <t>11 минут 17 секунд</t>
+  </si>
+  <si>
+    <t>5 Minutes Of Chess Grandmasters Giving Hilarious Answers To Interviews</t>
+  </si>
+  <si>
+    <t>101K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus Is DONE With Chess?</t>
+  </si>
+  <si>
+    <t>5 минут 43 секунды</t>
+  </si>
+  <si>
+    <t>Which Team Will Be CROWNED CHAMPION?! | 2024 Team Chess Battle FINAL</t>
+  </si>
+  <si>
+    <t>17K просмотров</t>
+  </si>
+  <si>
+    <t>It's OVER For Them</t>
+  </si>
+  <si>
+    <t>47K просмотров</t>
+  </si>
+  <si>
+    <t>22 минуты</t>
+  </si>
+  <si>
+    <t>Can ANYONE Beat This Superstar Chess Team?!</t>
+  </si>
+  <si>
+    <t>10K просмотров</t>
+  </si>
+  <si>
+    <t>These Chess Masters are STRUGGLING 💀</t>
+  </si>
+  <si>
+    <t>21K просмотров</t>
+  </si>
+  <si>
+    <t>34 минуты 29 секунд</t>
+  </si>
+  <si>
+    <t>The Top 5 BEST Chess Tricks To Use Against Your New Friends!</t>
+  </si>
+  <si>
+    <t>13K просмотров</t>
+  </si>
+  <si>
+    <t>Are Hikaru Nakamura and GothamChess The BEST Chess Teammates EVER?</t>
+  </si>
+  <si>
+    <t>169K просмотров</t>
+  </si>
+  <si>
+    <t>11 минут 13 секунд</t>
+  </si>
+  <si>
+    <t>Women's World Champion Faces Off Against Women’s World Blitz Champion!</t>
+  </si>
+  <si>
+    <t>Can This 15-Year-Old Break The Youngest UK Grandmaster Record?</t>
+  </si>
+  <si>
+    <t>9 минут 57 секунд</t>
+  </si>
+  <si>
+    <t>Grandmaster's Wild Mouse Slips But They Only Get Crazier</t>
+  </si>
+  <si>
+    <t>59K просмотров</t>
+  </si>
+  <si>
+    <t>Grandmaster Promotes Pawn To A KNIGHT To WIN?!</t>
+  </si>
+  <si>
+    <t>17 минут 29 секунд</t>
+  </si>
+  <si>
+    <t>World No.2 Has 166 bpm HEART RATE in TIE-BREAK | Levon Aronian vs Fabiano Caruana</t>
+  </si>
+  <si>
+    <t>25K просмотров</t>
+  </si>
+  <si>
+    <t>An Exclusive Look Inside Magnus Carlsen's Home!</t>
+  </si>
+  <si>
+    <t>779K просмотров</t>
+  </si>
+  <si>
+    <t>11 минут 28 секунд</t>
+  </si>
+  <si>
+    <t>Magnus Is Winning! Not Anymore?! Wait... What?!</t>
+  </si>
+  <si>
+    <t>5 Checkmates Chess ENGINES CAN'T Find!</t>
+  </si>
+  <si>
+    <t>114K просмотров</t>
+  </si>
+  <si>
+    <t>18 минут 43 секунды</t>
+  </si>
+  <si>
+    <t>Random Strangers In London TRY To Solve IMPOSSIBLE Chess Puzzles</t>
+  </si>
+  <si>
+    <t>66K просмотров</t>
+  </si>
+  <si>
+    <t>Best Chess Moments Of 2023</t>
+  </si>
+  <si>
+    <t>144K просмотров</t>
+  </si>
+  <si>
+    <t>22 минуты 38 секунд</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen on Cheating in Chess, Being the GOAT, and Retiring from the Game..</t>
+  </si>
+  <si>
+    <t>522K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen's Biggest Comeback EVER!?</t>
+  </si>
+  <si>
+    <t>261K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 26 секунд</t>
+  </si>
+  <si>
+    <t>7 Minutes Of Grandmasters LOSING On TIME</t>
+  </si>
+  <si>
+    <t>48K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus PERFECT???</t>
+  </si>
+  <si>
+    <t>11 минут</t>
+  </si>
+  <si>
+    <t>BAD CHESS ADVICE??? Grandmaster Reacts!</t>
+  </si>
+  <si>
+    <t>126K просмотров</t>
+  </si>
+  <si>
+    <t>GothamChess Forced To Answer Tough Personal Questions | LIE DETECTOR CHESS</t>
+  </si>
+  <si>
+    <t>994K просмотров</t>
+  </si>
+  <si>
+    <t>18 минут</t>
+  </si>
+  <si>
+    <t>Wesley So Plays The Youngest-Ever World Chess Champion!</t>
+  </si>
+  <si>
+    <t>56K просмотров</t>
+  </si>
+  <si>
+    <t>Grandmaster Wesley So Attempts BLINDFOLDED Blitz Chess Challenge</t>
+  </si>
+  <si>
+    <t>65K просмотров</t>
+  </si>
+  <si>
+    <t>5 минут 20 секунд</t>
+  </si>
+  <si>
+    <t>Fabiano Caruana STUNS Nodirbek Abdusattorov In Must Win Armageddon</t>
+  </si>
+  <si>
+    <t>15K просмотров</t>
+  </si>
+  <si>
+    <t>Can These Grandmasters Solve Our HARDEST Chess Puzzles?!?! 😰</t>
+  </si>
+  <si>
+    <t>689K просмотров</t>
+  </si>
+  <si>
+    <t>8 минут 52 секунды</t>
+  </si>
+  <si>
+    <t>Hikaru Nakamura Puts On EPIC Display During Intense Endgame</t>
+  </si>
+  <si>
+    <t>Hikaru Nakamura Fights For His Tournament Life</t>
+  </si>
+  <si>
+    <t>35K просмотров</t>
+  </si>
+  <si>
+    <t>9 минут 14 секунд</t>
+  </si>
+  <si>
+    <t>Hikaru Answers The Internet's Most Pressing Questions</t>
+  </si>
+  <si>
+    <t>305K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen vs. Alireza Firouzja Battle In A Wild Armageddon</t>
+  </si>
+  <si>
+    <t>10 минут 24 секунды</t>
+  </si>
+  <si>
+    <t>This Chess Prodigy Became The Youngest World Champion EVER!</t>
+  </si>
+  <si>
+    <t>Rapid Fire Questions With Grandmaster Wesley So</t>
+  </si>
+  <si>
+    <t>45K просмотров</t>
+  </si>
+  <si>
+    <t>39 минут 52 секунды</t>
+  </si>
+  <si>
+    <t>The Chess Phenom Wrongly Accused Of Cheating</t>
+  </si>
+  <si>
+    <t>GothamChess Gets ROASTED Playing Chili Chess 🥵🌶️</t>
+  </si>
+  <si>
+    <t>99K просмотров</t>
+  </si>
+  <si>
+    <t>11 минут 1 секунда</t>
+  </si>
+  <si>
+    <t>Wesley So vs. Magnus Carlsen! Is This The Game Of The YEAR?!?!</t>
+  </si>
+  <si>
+    <t>167K просмотров</t>
+  </si>
+  <si>
+    <t>How Chess.com Prevents Cheating At Chess Events</t>
+  </si>
+  <si>
+    <t>1 минута 52 секунды</t>
+  </si>
+  <si>
+    <t>Chess Grandmaster Gift Exchange Goes HILARIOUSLY Wrong</t>
+  </si>
+  <si>
+    <t>123K просмотров</t>
+  </si>
+  <si>
+    <t>Magnus Carlsen vs. Hikaru Nakamura's EPIC Armageddon Chess Battle</t>
+  </si>
+  <si>
+    <t>736K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 39 секунд</t>
+  </si>
+  <si>
+    <t>Does Magnus Carlsen REALLY Know Hikaru Nakamura?</t>
+  </si>
+  <si>
+    <t>314K просмотров</t>
+  </si>
+  <si>
+    <t>GothamChess Predicts Who Will Be Crowned Champion For The 2023 CCT!</t>
+  </si>
+  <si>
+    <t>4 минуты 39 секунд</t>
+  </si>
+  <si>
+    <t>Checkers is ATTACKING!</t>
+  </si>
+  <si>
+    <t>Does Hikaru Nakamura REALLY Know Magnus Carlsen?</t>
+  </si>
+  <si>
+    <t>214K просмотров</t>
+  </si>
+  <si>
+    <t>7 минут 12 секунд</t>
+  </si>
+  <si>
+    <t>Chess Grandmasters Raging At Bad Chess Moves</t>
+  </si>
+  <si>
+    <t>120K просмотров</t>
+  </si>
+  <si>
+    <t>Exclusive Look into Hikaru Nakamura's World Famous Office</t>
+  </si>
+  <si>
+    <t>254K просмотров</t>
+  </si>
+  <si>
+    <t>8 минут 11 секунд</t>
+  </si>
+  <si>
+    <t>We Asked Las Vegas Strangers About Chess</t>
+  </si>
+  <si>
+    <t>The Best Chess Players Over Time</t>
+  </si>
+  <si>
+    <t>190K просмотров</t>
+  </si>
+  <si>
+    <t>8 минут 5 секунд</t>
+  </si>
+  <si>
+    <t>New Carlos Alcaraz Bot On Chess.com Serves Up Epic Games</t>
+  </si>
+  <si>
+    <t>8,4K просмотров</t>
+  </si>
+  <si>
+    <t>Chess Masters Laughing At Bad Chess Moves</t>
+  </si>
+  <si>
+    <t>5 минут 5 секунд</t>
+  </si>
+  <si>
+    <t>Can AI Replace Magnus Carlsen?</t>
+  </si>
+  <si>
+    <t>Duolingo And Chess.com Join Forces For New Bots!</t>
+  </si>
+  <si>
     <t>196K просмотров</t>
   </si>
   <si>
-    <t>4:40</t>
-  </si>
-  <si>
-    <t>HIKARU vs #3 IN THE WORLD!!!</t>
-  </si>
-  <si>
-    <t>1 месяц назад</t>
-  </si>
-  <si>
-    <t>FABIANO OUTPLAYS STOCKFISH IN ANALYSIS!</t>
-  </si>
-  <si>
-    <t>137K просмотров</t>
-  </si>
-  <si>
-    <t>29:07</t>
-  </si>
-  <si>
-    <t>HIKARU ON BREAKING THE 2800 BARRIER IN CLASSICAL CHESS</t>
-  </si>
-  <si>
-    <t>MAGNUS ON THE ODDS OF LOSING HIS WORLD NO.1 SPOT</t>
-  </si>
-  <si>
-    <t>85K просмотров</t>
-  </si>
-  <si>
-    <t>16:52</t>
-  </si>
-  <si>
-    <t>PRAGG BEATS MAGNUS FOR THE 1ST TIME IN CLASSICAL CHESS!</t>
-  </si>
-  <si>
-    <t>Accused of Cheating by World Champions, Can He Prove Them Wrong?</t>
-  </si>
-  <si>
-    <t>57K просмотров</t>
-  </si>
-  <si>
-    <t>17:26</t>
-  </si>
-  <si>
-    <t>MAGNUS VS HIKARU ARMAGEDDON!!</t>
-  </si>
-  <si>
-    <t>HIKARU VS. FABI IN WILD ARMAGEDDON!</t>
-  </si>
-  <si>
-    <t>19K просмотров</t>
-  </si>
-  <si>
-    <t>9:38</t>
-  </si>
-  <si>
-    <t>🚨 MAGNUS VS DING! CURRENT VS FORMER WORLD CHAMP! ARMAGEDDON TIEBREAKER! 🚨</t>
-  </si>
-  <si>
-    <t>Can These Chess Grandmasters Ace This Simple Spelling Test??</t>
-  </si>
-  <si>
-    <t>93K просмотров</t>
-  </si>
-  <si>
-    <t>13:07</t>
-  </si>
-  <si>
-    <t>Magnus and Hikaru Face Off In A Historic Battle</t>
-  </si>
-  <si>
-    <t>The WILD Final Game Between Magnus And Alireza!</t>
-  </si>
-  <si>
-    <t>231K просмотров</t>
-  </si>
-  <si>
-    <t>16:48</t>
-  </si>
-  <si>
-    <t>Alireza: "I was lucky that Magnus got so tilted after game 4"</t>
-  </si>
-  <si>
-    <t>Vishy Answers The Web's Most Searched Questions!</t>
-  </si>
-  <si>
-    <t>12K просмотров</t>
-  </si>
-  <si>
-    <t>13:59</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen: "I knew if I won this match I would have two days off"</t>
-  </si>
-  <si>
-    <t>We Combined Disc Golf and Giant Chess!</t>
-  </si>
-  <si>
-    <t>22:41</t>
-  </si>
-  <si>
-    <t>5 Minutes Of Grandmasters Losing Their Minds To Crazy Moves</t>
-  </si>
-  <si>
-    <t>Magnus Forced to Answer Tough Personal Questions 🌶️ | LIE DETECTOR CHESS</t>
-  </si>
-  <si>
-    <t>150K просмотров</t>
-  </si>
-  <si>
-    <t>22:17</t>
-  </si>
-  <si>
-    <t>They Left Everything On The Board | Nepo vs. Fabi | Candidates 2024</t>
-  </si>
-  <si>
-    <t>Vaishali Opens Up About The Pressures of Chess Stardom In India</t>
-  </si>
-  <si>
-    <t>179K просмотров</t>
-  </si>
-  <si>
-    <t>12:31</t>
-  </si>
-  <si>
-    <t>Every Move From Pragg vs. Fabi | Candidates 2024 Round 13</t>
-  </si>
-  <si>
-    <t>Final Heart-stopping Moments From Gukesh vs. Alireza | Candidates 2024</t>
-  </si>
-  <si>
-    <t>185K просмотров</t>
-  </si>
-  <si>
-    <t>11:31</t>
-  </si>
-  <si>
-    <t>Every Move from Hikaru vs. Alireza | Candidates 2024 Round 12</t>
-  </si>
-  <si>
-    <t>GothamChess And Vidit Dive Into The Emotions Of The Candidates!</t>
-  </si>
-  <si>
-    <t>139K просмотров</t>
-  </si>
-  <si>
-    <t>21:46</t>
-  </si>
-  <si>
-    <t>What An Endgame 🤯 | Vidit vs. Nepo</t>
-  </si>
-  <si>
-    <t>Did GothamChess And Nijat Just Become Best Friends?!</t>
-  </si>
-  <si>
-    <t>38K просмотров</t>
-  </si>
-  <si>
-    <t>15:38</t>
-  </si>
-  <si>
-    <t>Chess is BRUTAL! | Alireza vs. Gukesh | Candidates 2024</t>
-  </si>
-  <si>
-    <t>The Brilliant Final Moments of Hikaru vs. Nepo | Candidates 2024</t>
-  </si>
-  <si>
-    <t>16:53</t>
-  </si>
-  <si>
-    <t>The Stressful Final 5 Minutes Of Vidit vs. Alireza | Candidates 2024</t>
-  </si>
-  <si>
-    <t>GothamChess and Pragg Finally Meet in Exclusive Interview!</t>
-  </si>
-  <si>
-    <t>43K просмотров</t>
-  </si>
-  <si>
-    <t>17:44</t>
-  </si>
-  <si>
-    <t>Nepo Vs. Pragg | Game 6 | Candidates 2024</t>
-  </si>
-  <si>
-    <t>The Wild Final 10 Minutes Of Hikaru vs. Alireza | Candidates 2024</t>
-  </si>
-  <si>
-    <t>23K просмотров</t>
-  </si>
-  <si>
-    <t>4:18</t>
-  </si>
-  <si>
-    <t>Vishy's Exclusive Dinner with Indian Candidates ft. Pragg, Gukesh, Vaishali, Humpy</t>
-  </si>
-  <si>
-    <t>Fabiano's Fight To Be The No. 1 Chess Player In The World</t>
-  </si>
-  <si>
-    <t>38:08</t>
-  </si>
-  <si>
-    <t>Chess.com but it's IRL</t>
-  </si>
-  <si>
-    <t>Vaishali's Dreams Of Becoming A Chess World Champion</t>
-  </si>
-  <si>
-    <t>69K просмотров</t>
-  </si>
-  <si>
-    <t>14:46</t>
-  </si>
-  <si>
-    <t>We Finally Updated Chess (APRIL FOOLS!)</t>
-  </si>
-  <si>
-    <t>This Impossible Puzzle Stumped 99% Of Chess.com Users!</t>
-  </si>
-  <si>
-    <t>39K просмотров</t>
-  </si>
-  <si>
-    <t>13:12</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen Ranks The Candidates Players! 🌶️</t>
-  </si>
-  <si>
-    <t>The Craziest Moments From The Candidates!</t>
-  </si>
-  <si>
-    <t>82K просмотров</t>
-  </si>
-  <si>
-    <t>Gukesh Fights Back Against Anish Giri To Find A Huge Win!</t>
-  </si>
-  <si>
-    <t>Can This 17-Year-Old Make Chess History and Win a Ticket to the World Championship?</t>
-  </si>
-  <si>
-    <t>77K просмотров</t>
-  </si>
-  <si>
-    <t>7:24</t>
-  </si>
-  <si>
-    <t>Game 1 Of The Drama Filled Match Between Anish Giri and Gukesh</t>
-  </si>
-  <si>
-    <t>2 месяца назад</t>
-  </si>
-  <si>
-    <t>The Chess Game That Changed Wesley So's Life</t>
-  </si>
-  <si>
-    <t>11:17</t>
-  </si>
-  <si>
-    <t>5 Minutes Of Chess Grandmasters Giving Hilarious Answers To Interviews</t>
-  </si>
-  <si>
-    <t>Magnus Is DONE With Chess?</t>
-  </si>
-  <si>
-    <t>200K просмотров</t>
-  </si>
-  <si>
-    <t>5:43</t>
-  </si>
-  <si>
-    <t>Which Team Will Be CROWNED CHAMPION?! | 2024 Team Chess Battle FINAL</t>
-  </si>
-  <si>
-    <t>It's OVER For Them</t>
-  </si>
-  <si>
-    <t>944K просмотров</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>Can ANYONE Beat This Superstar Chess Team?!</t>
-  </si>
-  <si>
-    <t>These Chess Masters are STRUGGLING 💀</t>
-  </si>
-  <si>
-    <t>90K просмотров</t>
-  </si>
-  <si>
-    <t>34:29</t>
-  </si>
-  <si>
-    <t>The Top 5 BEST Chess Tricks To Use Against Your New Friends!</t>
-  </si>
-  <si>
-    <t>Are Hikaru Nakamura and GothamChess The BEST Chess Teammates EVER?</t>
-  </si>
-  <si>
-    <t>55K просмотров</t>
-  </si>
-  <si>
-    <t>11:13</t>
-  </si>
-  <si>
-    <t>Women's World Champion Faces Off Against Women’s World Blitz Champion!</t>
-  </si>
-  <si>
-    <t>Can This 15-Year-Old Break The Youngest UK Grandmaster Record?</t>
-  </si>
-  <si>
-    <t>9,8K просмотров</t>
-  </si>
-  <si>
-    <t>9:57</t>
-  </si>
-  <si>
-    <t>Grandmaster's Wild Mouse Slips But They Only Get Crazier</t>
-  </si>
-  <si>
-    <t>Grandmaster Promotes Pawn To A KNIGHT To WIN?!</t>
-  </si>
-  <si>
-    <t>72K просмотров</t>
-  </si>
-  <si>
-    <t>17:29</t>
-  </si>
-  <si>
-    <t>World No.2 Has 166 bpm HEART RATE in TIE-BREAK | Levon Aronian vs Fabiano Caruana</t>
-  </si>
-  <si>
-    <t>An Exclusive Look Inside Magnus Carlsen's Home!</t>
-  </si>
-  <si>
-    <t>24K просмотров</t>
-  </si>
-  <si>
-    <t>11:28</t>
-  </si>
-  <si>
-    <t>Magnus Is Winning! Not Anymore?! Wait... What?!</t>
-  </si>
-  <si>
-    <t>5 Checkmates Chess ENGINES CAN'T Find!</t>
-  </si>
-  <si>
-    <t>83K просмотров</t>
-  </si>
-  <si>
-    <t>18:43</t>
-  </si>
-  <si>
-    <t>Random Strangers In London TRY To Solve IMPOSSIBLE Chess Puzzles</t>
-  </si>
-  <si>
-    <t>Best Chess Moments Of 2023</t>
-  </si>
-  <si>
-    <t>62K просмотров</t>
-  </si>
-  <si>
-    <t>22:38</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen on Cheating in Chess, Being the GOAT, and Retiring from the Game..</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen's Biggest Comeback EVER!?</t>
-  </si>
-  <si>
-    <t>73K просмотров</t>
-  </si>
-  <si>
-    <t>13:26</t>
-  </si>
-  <si>
-    <t>7 Minutes Of Grandmasters LOSING On TIME</t>
-  </si>
-  <si>
-    <t>3 месяца назад</t>
-  </si>
-  <si>
-    <t>Magnus PERFECT???</t>
-  </si>
-  <si>
-    <t>98K просмотров</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>BAD CHESS ADVICE??? Grandmaster Reacts!</t>
-  </si>
-  <si>
-    <t>GothamChess Forced To Answer Tough Personal Questions | LIE DETECTOR CHESS</t>
-  </si>
-  <si>
-    <t>97K просмотров</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>Wesley So Plays The Youngest-Ever World Chess Champion!</t>
-  </si>
-  <si>
-    <t>Grandmaster Wesley So Attempts BLINDFOLDED Blitz Chess Challenge</t>
-  </si>
-  <si>
-    <t>41K просмотров</t>
-  </si>
-  <si>
-    <t>5:20</t>
-  </si>
-  <si>
-    <t>Fabiano Caruana STUNS Nodirbek Abdusattorov In Must Win Armageddon</t>
-  </si>
-  <si>
-    <t>Can These Grandmasters Solve Our HARDEST Chess Puzzles?!?! 😰</t>
-  </si>
-  <si>
-    <t>238K просмотров</t>
-  </si>
-  <si>
-    <t>8:52</t>
-  </si>
-  <si>
-    <t>Hikaru Nakamura Puts On EPIC Display During Intense Endgame</t>
-  </si>
-  <si>
-    <t>Hikaru Nakamura Fights For His Tournament Life</t>
-  </si>
-  <si>
-    <t>9:14</t>
-  </si>
-  <si>
-    <t>Hikaru Answers The Internet's Most Pressing Questions</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen vs. Alireza Firouzja Battle In A Wild Armageddon</t>
-  </si>
-  <si>
-    <t>199K просмотров</t>
-  </si>
-  <si>
-    <t>10:24</t>
-  </si>
-  <si>
-    <t>This Chess Prodigy Became The Youngest World Champion EVER!</t>
-  </si>
-  <si>
-    <t>Rapid Fire Questions With Grandmaster Wesley So</t>
-  </si>
-  <si>
-    <t>758K просмотров</t>
-  </si>
-  <si>
-    <t>39:52</t>
-  </si>
-  <si>
-    <t>The Chess Phenom Wrongly Accused Of Cheating</t>
-  </si>
-  <si>
-    <t>GothamChess Gets ROASTED Playing Chili Chess 🥵🌶️</t>
-  </si>
-  <si>
-    <t>32K просмотров</t>
-  </si>
-  <si>
-    <t>11:01</t>
-  </si>
-  <si>
-    <t>Wesley So vs. Magnus Carlsen! Is This The Game Of The YEAR?!?!</t>
-  </si>
-  <si>
-    <t>How Chess.com Prevents Cheating At Chess Events</t>
-  </si>
-  <si>
-    <t>1:52</t>
-  </si>
-  <si>
-    <t>Chess Grandmaster Gift Exchange Goes HILARIOUSLY Wrong</t>
-  </si>
-  <si>
-    <t>Magnus Carlsen vs. Hikaru Nakamura's EPIC Armageddon Chess Battle</t>
-  </si>
-  <si>
-    <t>13:39</t>
-  </si>
-  <si>
-    <t>Does Magnus Carlsen REALLY Know Hikaru Nakamura?</t>
-  </si>
-  <si>
-    <t>GothamChess Predicts Who Will Be Crowned Champion For The 2023 CCT!</t>
-  </si>
-  <si>
-    <t>159K просмотров</t>
-  </si>
-  <si>
-    <t>4:39</t>
-  </si>
-  <si>
-    <t>Checkers is ATTACKING!</t>
-  </si>
-  <si>
-    <t>Does Hikaru Nakamura REALLY Know Magnus Carlsen?</t>
-  </si>
-  <si>
-    <t>30K просмотров</t>
-  </si>
-  <si>
-    <t>7:12</t>
-  </si>
-  <si>
-    <t>Chess Grandmasters Raging At Bad Chess Moves</t>
-  </si>
-  <si>
-    <t>Exclusive Look into Hikaru Nakamura's World Famous Office</t>
-  </si>
-  <si>
-    <t>1M просмотров</t>
-  </si>
-  <si>
-    <t>8:11</t>
-  </si>
-  <si>
-    <t>We Asked Las Vegas Strangers About Chess</t>
-  </si>
-  <si>
-    <t>The Best Chess Players Over Time</t>
-  </si>
-  <si>
-    <t>112K просмотров</t>
-  </si>
-  <si>
-    <t>8:05</t>
-  </si>
-  <si>
-    <t>New Carlos Alcaraz Bot On Chess.com Serves Up Epic Games</t>
-  </si>
-  <si>
-    <t>Chess Masters Laughing At Bad Chess Moves</t>
-  </si>
-  <si>
-    <t>16K просмотров</t>
-  </si>
-  <si>
-    <t>5:05</t>
-  </si>
-  <si>
-    <t>Can AI Replace Magnus Carlsen?</t>
-  </si>
-  <si>
-    <t>Duolingo And Chess.com Join Forces For New Bots!</t>
-  </si>
-  <si>
-    <t>28K просмотров</t>
-  </si>
-  <si>
-    <t>10:05</t>
+    <t>10 минут 5 секунд</t>
   </si>
   <si>
     <t>Chess.com Gets Real About Cheating In Chess</t>
   </si>
   <si>
+    <t>107K просмотров</t>
+  </si>
+  <si>
     <t>Chess Got Weird at Twitchcon</t>
   </si>
   <si>
-    <t>20K просмотров</t>
-  </si>
-  <si>
-    <t>6:54</t>
+    <t>6 минут 54 секунды</t>
   </si>
   <si>
     <t>Chess.com Reacts To Hilarious Support Emails</t>
@@ -700,7 +787,7 @@
     <t>Learn How to Play Our New Variant Spell Chess With 5 Quick Tips</t>
   </si>
   <si>
-    <t>17:08</t>
+    <t>17 минут 8 секунд</t>
   </si>
   <si>
     <t>How to Avoid the 10 Most Common Mistakes in Chess</t>
@@ -709,70 +796,85 @@
     <t>Chess Grandmasters Missing Checkmate-In-1</t>
   </si>
   <si>
-    <t>101K просмотров</t>
-  </si>
-  <si>
-    <t>5:11</t>
+    <t>71K просмотров</t>
+  </si>
+  <si>
+    <t>5 минут 11 секунд</t>
   </si>
   <si>
     <t>Five-time World Chess Champion Shows Off His CRAZY Trophy Room</t>
   </si>
   <si>
+    <t>316K просмотров</t>
+  </si>
+  <si>
     <t>GothamChess, Eric Rosen And More Play Spell Chess!</t>
   </si>
   <si>
-    <t>13:40</t>
+    <t>18K просмотров</t>
+  </si>
+  <si>
+    <t>13 минут 40 секунд</t>
   </si>
   <si>
     <t>Magnus Carlsen Gives His Best Chess Advice</t>
   </si>
   <si>
-    <t>4 месяца назад</t>
+    <t>51K просмотров</t>
   </si>
   <si>
     <t>How Well Do Grandmasters Know Their Chess History?</t>
   </si>
   <si>
-    <t>17K просмотров</t>
-  </si>
-  <si>
-    <t>39:12</t>
+    <t>37K просмотров</t>
+  </si>
+  <si>
+    <t>39 минут 12 секунд</t>
   </si>
   <si>
     <t>Viswanathan Anand On India's Past, Present, And Bright Future In Chess</t>
   </si>
   <si>
+    <t>33K просмотров</t>
+  </si>
+  <si>
     <t>Grandmasters Playing Troll Chess Openings, But They Only Get Crazier</t>
   </si>
   <si>
-    <t>47K просмотров</t>
-  </si>
-  <si>
-    <t>49:39</t>
+    <t>40K просмотров</t>
+  </si>
+  <si>
+    <t>49 минут 39 секунд</t>
   </si>
   <si>
     <t>8-Year-Old Chess Prodigy Challenges 79-Year-Old British Chess Champion</t>
   </si>
   <si>
+    <t>508K просмотров</t>
+  </si>
+  <si>
     <t>Magnus Carlsen Shows Off His Creativity In Speed Chess | 2023 Speed Chess Championship Highlights</t>
   </si>
   <si>
-    <t>10K просмотров</t>
-  </si>
-  <si>
-    <t>41:44</t>
+    <t>34K просмотров</t>
+  </si>
+  <si>
+    <t>41 минута 44 секунды</t>
   </si>
   <si>
     <t>PSA: Chess Is Taking Over Schools</t>
   </si>
   <si>
+    <t>29K просмотров</t>
+  </si>
+  <si>
     <t>Fabiano Caruana Pulls Off An INCREDIBLE Comeback | 2023 Speed Chess Championship Highlights</t>
   </si>
   <si>
-    <t>21K просмотров</t>
-  </si>
-  <si>
-    <t>5:13</t>
+    <t>11K просмотров</t>
+  </si>
+  <si>
+    <t>5 минут 13 секунд</t>
   </si>
   <si>
     <t>Chess.com Updates Chess</t>
@@ -781,22 +883,19 @@
     <t>Alireza Firouzja's Lightning FAST Speed | Speed Chess Championship 2023 Highlights</t>
   </si>
   <si>
-    <t>13K просмотров</t>
-  </si>
-  <si>
-    <t>7:04</t>
+    <t>7 минут 4 секунды</t>
   </si>
   <si>
     <t>Chess.com Reacts To The Craziest Emails From Cheaters</t>
   </si>
   <si>
+    <t>81K просмотров</t>
+  </si>
+  <si>
     <t>Hikaru Shows Why He's A Speed Chess Demon | Speed Chess Championship 2023 Highlights</t>
   </si>
   <si>
-    <t>169K просмотров</t>
-  </si>
-  <si>
-    <t>24:10</t>
+    <t>24 минуты 10 секунд</t>
   </si>
   <si>
     <t>Chess.com And Clash Of Clans Team Up For An Epic Crossover!</t>
@@ -805,16 +904,25 @@
     <t>Get Ready To Clash With Our New Chess Bots!</t>
   </si>
   <si>
-    <t>8:30</t>
+    <t>27K просмотров</t>
+  </si>
+  <si>
+    <t>8 минут 30 секунд</t>
   </si>
   <si>
     <t>Chess Masters Attempt Our New Variant in Spell Chess</t>
   </si>
   <si>
+    <t>118K просмотров</t>
+  </si>
+  <si>
     <t>Chess Opening Traps That ACTUALLY Work!</t>
   </si>
   <si>
-    <t>7:47</t>
+    <t>146K просмотров</t>
+  </si>
+  <si>
+    <t>7 минут 47 секунд</t>
   </si>
   <si>
     <t>The City Of Human Chess | Official Trailer</t>
@@ -823,19 +931,19 @@
     <t>The Best Moments From Frank vs. CDawg | Pogchamps 5 Championship Bracket Final</t>
   </si>
   <si>
-    <t>59K просмотров</t>
-  </si>
-  <si>
-    <t>4:33</t>
+    <t>4 минуты 33 секунды</t>
   </si>
   <si>
     <t>Wirtual vs. QTCinderella | Pogchamps 5 Consolation Finals</t>
   </si>
   <si>
+    <t>52K просмотров</t>
+  </si>
+  <si>
     <t>GothamChess Predicts Terrible Chess Moves</t>
   </si>
   <si>
-    <t>4:23</t>
+    <t>4 минуты 23 секунды</t>
   </si>
   <si>
     <t>Chess Grandmaster vs. ALL Of Twitchcon</t>
@@ -844,58 +952,67 @@
     <t>The Top 5 Best Chess Openings For Aggressive Beginners</t>
   </si>
   <si>
-    <t>25K просмотров</t>
-  </si>
-  <si>
-    <t>9:03</t>
+    <t>95K просмотров</t>
+  </si>
+  <si>
+    <t>9 минут 3 секунды</t>
   </si>
   <si>
     <t>Hikaru Nakamura Battles Against Magnus Carlsen's Speed</t>
   </si>
   <si>
+    <t>2,5M просмотров</t>
+  </si>
+  <si>
     <t>Chess Games So Good The Opponent Has To Applaud</t>
   </si>
   <si>
-    <t>778K просмотров</t>
-  </si>
-  <si>
-    <t>4:09</t>
+    <t>64K просмотров</t>
+  </si>
+  <si>
+    <t>4 минуты 9 секунд</t>
   </si>
   <si>
     <t>We Asked Strangers In Norway About Chess</t>
   </si>
   <si>
+    <t>61K просмотров</t>
+  </si>
+  <si>
     <t>xQc Pulls Off The UNTHINKABLE vs. Papaplatte</t>
   </si>
   <si>
-    <t>18:50</t>
+    <t>115K просмотров</t>
+  </si>
+  <si>
+    <t>18 минут 50 секунд</t>
   </si>
   <si>
     <t>Magnus Carlsen's EPIC Time Scramble vs. Mamedyarov</t>
   </si>
   <si>
+    <t>44K просмотров</t>
+  </si>
+  <si>
     <t>Frank Unlocks A New Level To His Chess Game</t>
   </si>
   <si>
-    <t>114K просмотров</t>
-  </si>
-  <si>
-    <t>13:22</t>
+    <t>13 минут 22 секунды</t>
   </si>
   <si>
     <t>xQc vs. Tyler1 | Full Match | Pogchamps 5 | Chess Unlike Anything You've Seen</t>
   </si>
   <si>
-    <t>5 месяцев назад</t>
+    <t>46K просмотров</t>
   </si>
   <si>
     <t>xQc And Tyler1 Roast Each Other For 12 Minutes</t>
   </si>
   <si>
-    <t>66K просмотров</t>
-  </si>
-  <si>
-    <t>6:31</t>
+    <t>140K просмотров</t>
+  </si>
+  <si>
+    <t>6 минут 31 секунда</t>
   </si>
   <si>
     <t>xQc Thinks He Is Hikaru</t>
@@ -904,10 +1021,7 @@
     <t>xQc Wants Revenge At Pogchamps</t>
   </si>
   <si>
-    <t>144K просмотров</t>
-  </si>
-  <si>
-    <t>13:20</t>
+    <t>13 минут 20 секунд</t>
   </si>
   <si>
     <t>CDawgVA Pulls Out The Chess Coloring Book After Defeating Frank</t>
@@ -1385,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1393,450 +1507,450 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="C47" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s">
         <v>30</v>
@@ -1844,10 +1958,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -1855,1058 +1969,1058 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="B73" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C74" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="C75" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="C78" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="B80" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="C81" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="C82" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="C83" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="C84" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="C85" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C86" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C87" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>203</v>
       </c>
       <c r="C88" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
       <c r="C89" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>99</v>
       </c>
       <c r="C90" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="B92" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="C92" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="B93" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="C93" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="B94" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="C94" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="B95" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="C95" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="C96" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="B97" t="s">
-        <v>161</v>
+        <v>222</v>
       </c>
       <c r="C97" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="B98" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
       <c r="C98" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="B99" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>86</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="B101" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="C102" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
       <c r="B103" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="C103" t="s">
-        <v>205</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="B104" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="C104" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="B105" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="C106" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="B107" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="C107" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="B109" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="B110" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="C110" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="B111" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="B112" t="s">
-        <v>224</v>
+        <v>131</v>
       </c>
       <c r="C112" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="B113" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="C113" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>227</v>
+        <v>256</v>
       </c>
       <c r="B114" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
       <c r="C114" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="B116" t="s">
-        <v>231</v>
+        <v>260</v>
       </c>
       <c r="C116" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>233</v>
+        <v>262</v>
       </c>
       <c r="B117" t="s">
-        <v>161</v>
+        <v>263</v>
       </c>
       <c r="C117" t="s">
-        <v>232</v>
+        <v>261</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="B118" t="s">
-        <v>150</v>
+        <v>265</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="B119" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="C119" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>238</v>
+        <v>269</v>
       </c>
       <c r="B120" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
       <c r="C120" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>273</v>
       </c>
       <c r="C121" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="B122" t="s">
-        <v>243</v>
+        <v>275</v>
       </c>
       <c r="C122" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="C123" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="B124" t="s">
-        <v>247</v>
+        <v>280</v>
       </c>
       <c r="C124" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>249</v>
+        <v>282</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
       <c r="C125" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="B126" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="C126" t="s">
-        <v>252</v>
+        <v>286</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
       <c r="B127" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="C127" t="s">
-        <v>252</v>
+        <v>286</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>288</v>
       </c>
       <c r="B128" t="s">
-        <v>255</v>
+        <v>147</v>
       </c>
       <c r="C128" t="s">
-        <v>256</v>
+        <v>289</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="B129" t="s">
-        <v>237</v>
+        <v>291</v>
       </c>
       <c r="C129" t="s">
-        <v>256</v>
+        <v>289</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="B130" t="s">
-        <v>259</v>
+        <v>7</v>
       </c>
       <c r="C130" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="B131" t="s">
-        <v>237</v>
+        <v>149</v>
       </c>
       <c r="C131" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>262</v>
+        <v>295</v>
       </c>
       <c r="B132" t="s">
-        <v>50</v>
+        <v>296</v>
       </c>
       <c r="C132" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>264</v>
+        <v>298</v>
       </c>
       <c r="B133" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
       <c r="C133" t="s">
-        <v>263</v>
+        <v>297</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>265</v>
+        <v>300</v>
       </c>
       <c r="B134" t="s">
-        <v>50</v>
+        <v>301</v>
       </c>
       <c r="C134" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="B135" t="s">
-        <v>237</v>
+        <v>37</v>
       </c>
       <c r="C135" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="B136" t="s">
-        <v>269</v>
+        <v>183</v>
       </c>
       <c r="C136" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>271</v>
+        <v>306</v>
       </c>
       <c r="B137" t="s">
-        <v>237</v>
+        <v>307</v>
       </c>
       <c r="C137" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="B138" t="s">
-        <v>62</v>
+        <v>222</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="B139" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
       <c r="C139" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>275</v>
+        <v>311</v>
       </c>
       <c r="B140" t="s">
-        <v>276</v>
+        <v>312</v>
       </c>
       <c r="C140" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>278</v>
+        <v>314</v>
       </c>
       <c r="B141" t="s">
-        <v>237</v>
+        <v>315</v>
       </c>
       <c r="C141" t="s">
-        <v>277</v>
+        <v>313</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>279</v>
+        <v>316</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>317</v>
       </c>
       <c r="C142" t="s">
-        <v>281</v>
+        <v>318</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
+        <v>320</v>
       </c>
       <c r="C143" t="s">
-        <v>281</v>
+        <v>318</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="B144" t="s">
-        <v>224</v>
+        <v>322</v>
       </c>
       <c r="C144" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="B145" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="C145" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>286</v>
+        <v>326</v>
       </c>
       <c r="B146" t="s">
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="C146" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>289</v>
+        <v>328</v>
       </c>
       <c r="B147" t="s">
-        <v>290</v>
+        <v>329</v>
       </c>
       <c r="C147" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>291</v>
+        <v>330</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>331</v>
       </c>
       <c r="C148" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>294</v>
+        <v>333</v>
       </c>
       <c r="B149" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="C149" t="s">
-        <v>293</v>
+        <v>332</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>295</v>
+        <v>334</v>
       </c>
       <c r="B150" t="s">
-        <v>296</v>
+        <v>37</v>
       </c>
       <c r="C150" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="B151" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C151" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>